<commit_message>
fixes undefined for chair
</commit_message>
<xml_diff>
--- a/conference-app/sample programmes/smaller-5.xlsx
+++ b/conference-app/sample programmes/smaller-5.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="62">
   <si>
     <t xml:space="preserve">Title</t>
   </si>
@@ -201,12 +201,6 @@
   </si>
   <si>
     <t xml:space="preserve">Closure Planning and Stakeholders</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D Jasper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rio Tinto</t>
   </si>
   <si>
     <t xml:space="preserve">Hello world</t>
@@ -415,8 +409,8 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -689,7 +683,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
@@ -699,7 +693,9 @@
       <c r="C14" s="3" t="n">
         <v>43713.4791666667</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="3" t="n">
+        <v>43713.4798611111</v>
+      </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
@@ -745,8 +741,8 @@
   </sheetPr>
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -948,7 +944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
         <v>4</v>
       </c>
@@ -958,12 +954,8 @@
       <c r="C8" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>61</v>
-      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
       <c r="F8" s="4" t="n">
         <v>2</v>
       </c>
@@ -984,6 +976,9 @@
       <c r="B9" s="0" t="n">
         <v>8</v>
       </c>
+      <c r="C9" s="0" t="s">
+        <v>55</v>
+      </c>
       <c r="F9" s="0" t="n">
         <v>1</v>
       </c>
@@ -1002,10 +997,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>39</v>

</xml_diff>